<commit_message>
adding validation tests and refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/__files/datafile_output.xlsx
+++ b/src/test/resources/__files/datafile_output.xlsx
@@ -13,18 +13,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
+  <si>
+    <t>testing</t>
+  </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
     <t>error message</t>
   </si>
   <si>
     <t>success message</t>
+  </si>
+  <si>
+    <t>aaaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -80,7 +83,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="n">
@@ -92,10 +95,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="n">
@@ -107,12 +110,14 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4"/>
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" t="n">
         <v>1234.0</v>
       </c>
@@ -122,14 +127,14 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -137,10 +142,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="n">
@@ -148,6 +153,21 @@
       </c>
       <c r="F6" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -164,83 +184,103 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>1234.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1234.0</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.0</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3" t="n">
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="n">
-        <v>1234.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1234.0</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3.0</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>1</v>
+      <c r="A4" t="n">
+        <v>4.0</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="n">
-        <v>1234.0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1234.0</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1234.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>6.0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1234.0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>8.0</v>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1234.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>